<commit_message>
SPI_Master progress and updated docs
</commit_message>
<xml_diff>
--- a/Documentation/Project Schedule.xlsx
+++ b/Documentation/Project Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\axi2spi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843AAE9E-9952-4B53-BEDD-36A5343CE7F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95715DF-962B-4759-B9B3-C156AB3697BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Project Stage</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>FPGA testing</t>
+  </si>
+  <si>
+    <t>d1b4657</t>
   </si>
 </sst>
 </file>
@@ -684,6 +687,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -702,6 +709,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -720,28 +739,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1106,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1118,11 +1121,11 @@
       <c r="E2" s="15">
         <v>43963</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="55">
         <v>43963</v>
       </c>
       <c r="G2" s="30"/>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="45" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="32" t="s">
@@ -1133,7 +1136,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1146,9 +1149,9 @@
       <c r="E3" s="12">
         <v>43961</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="44"/>
+      <c r="H3" s="46"/>
       <c r="I3" s="33" t="s">
         <v>17</v>
       </c>
@@ -1157,7 +1160,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1168,9 +1171,9 @@
       <c r="E4" s="13">
         <v>43963</v>
       </c>
-      <c r="F4" s="50"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="44"/>
+      <c r="H4" s="46"/>
       <c r="I4" s="34" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1182,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1190,9 +1193,9 @@
       <c r="E5" s="14">
         <v>43961</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="31"/>
-      <c r="H5" s="45"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="35" t="s">
         <v>24</v>
       </c>
@@ -1201,7 +1204,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1214,11 +1217,11 @@
       <c r="E6" s="13">
         <v>43963</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="58">
         <v>43963</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="45" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="36" t="s">
@@ -1229,7 +1232,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
@@ -1240,9 +1243,9 @@
       <c r="E7" s="13">
         <v>43963</v>
       </c>
-      <c r="F7" s="50"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="44"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="37" t="s">
         <v>32</v>
       </c>
@@ -1251,7 +1254,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1262,12 +1265,12 @@
       <c r="E8" s="13">
         <v>43963</v>
       </c>
-      <c r="F8" s="50"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="44"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1278,12 +1281,12 @@
       <c r="E9" s="13">
         <v>43963</v>
       </c>
-      <c r="F9" s="50"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="45"/>
+      <c r="H9" s="47"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1296,7 +1299,7 @@
       <c r="E10" s="20">
         <v>43965</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="59">
         <v>43966</v>
       </c>
       <c r="G10" s="30"/>
@@ -1305,7 +1308,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
@@ -1316,14 +1319,14 @@
       <c r="E11" s="21">
         <v>43965</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="3"/>
       <c r="H11" s="40" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1332,12 +1335,12 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="3"/>
       <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
@@ -1348,7 +1351,7 @@
       <c r="E13" s="22">
         <v>43966</v>
       </c>
-      <c r="F13" s="54"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="3"/>
       <c r="H13" s="40" t="s">
         <v>44</v>
@@ -1356,7 +1359,7 @@
       <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
@@ -1367,7 +1370,7 @@
       <c r="E14" s="38">
         <v>43969</v>
       </c>
-      <c r="F14" s="54"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="3" t="s">
         <v>46</v>
       </c>
@@ -1376,7 +1379,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1387,14 +1390,14 @@
       <c r="E15" s="22">
         <v>43966</v>
       </c>
-      <c r="F15" s="54"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="3"/>
       <c r="H15" s="40" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="48" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1405,14 +1408,14 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="55">
+      <c r="F16" s="51">
         <v>43978</v>
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="39"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="2" t="s">
         <v>53</v>
       </c>
@@ -1421,12 +1424,12 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="56"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="3"/>
       <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="2" t="s">
         <v>54</v>
       </c>
@@ -1437,12 +1440,14 @@
       <c r="E18" s="21">
         <v>43977</v>
       </c>
-      <c r="F18" s="56"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="40"/>
+      <c r="H18" s="40" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1453,14 +1458,14 @@
       <c r="E19" s="21">
         <v>43969</v>
       </c>
-      <c r="F19" s="56"/>
+      <c r="F19" s="52"/>
       <c r="G19" s="3"/>
       <c r="H19" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="2" t="s">
         <v>57</v>
       </c>
@@ -1469,12 +1474,12 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="57"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="3"/>
       <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
@@ -1483,12 +1488,12 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="57"/>
+      <c r="F21" s="53"/>
       <c r="G21" s="3"/>
       <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
@@ -1496,10 +1501,10 @@
         <v>10</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="62">
+      <c r="E22" s="44">
         <v>43977</v>
       </c>
-      <c r="F22" s="58"/>
+      <c r="F22" s="54"/>
       <c r="G22" s="3"/>
       <c r="H22" s="41"/>
     </row>
@@ -1515,14 +1520,14 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="59">
+      <c r="F23" s="43">
         <v>43978</v>
       </c>
       <c r="G23" s="30"/>
       <c r="H23" s="40"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="48" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1531,45 +1536,45 @@
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="60">
+      <c r="F24" s="61">
         <v>43978</v>
       </c>
       <c r="G24" s="30"/>
       <c r="H24" s="39"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="60"/>
+      <c r="F25" s="61"/>
       <c r="G25" s="3"/>
       <c r="H25" s="40"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="60"/>
+      <c r="F26" s="61"/>
       <c r="G26" s="3"/>
       <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="61"/>
+      <c r="F27" s="62"/>
       <c r="G27" s="31"/>
       <c r="H27" s="41"/>
     </row>
@@ -1593,12 +1598,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1748,15 +1750,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{837235E1-7EB7-428A-9D4E-2E36B6940D1C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC183E54-2C7F-447F-9F20-20916199F4FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1780,10 +1786,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC183E54-2C7F-447F-9F20-20916199F4FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{837235E1-7EB7-428A-9D4E-2E36B6940D1C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>